<commit_message>
New Effort Chart created
</commit_message>
<xml_diff>
--- a/Chart.xlsx
+++ b/Chart.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanf\Desktop\School\Sem 3.2\ETI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C9A280-CA18-44F0-B97F-03E73FC82DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D17952-A8FD-4BA9-BC8A-72FE0F466C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="2175" windowWidth="22545" windowHeight="12315" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13830" yWindow="2190" windowWidth="22545" windowHeight="12315" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BurnUp Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Effort Chart" sheetId="2" r:id="rId2"/>
-    <sheet name="Effort Description" sheetId="3" r:id="rId3"/>
+    <sheet name="Effort Descriptions" sheetId="4" r:id="rId3"/>
+    <sheet name="do not refer" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Sprint</t>
-  </si>
-  <si>
-    <t>Story Points</t>
   </si>
   <si>
     <t>Total Story Points</t>
@@ -111,6 +109,36 @@
   </si>
   <si>
     <t xml:space="preserve">Pass/Fail Test Case </t>
+  </si>
+  <si>
+    <t>Story Points Completed</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Test Cases Created</t>
+  </si>
+  <si>
+    <t>Test Cases Passed</t>
+  </si>
+  <si>
+    <t>Integration tests passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual (Integration) Time Taken </t>
+  </si>
+  <si>
+    <t>TDD Coding Time Taken</t>
+  </si>
+  <si>
+    <t>Integration Time Taken</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Time Taken units:</t>
   </si>
 </sst>
 </file>
@@ -196,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -205,6 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,13 +242,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFF66CC"/>
+      <color rgb="FF00FFFF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FFFFFF66"/>
       <color rgb="FFCCFFFF"/>
-      <color rgb="FF00FFFF"/>
       <color rgb="FFFFCCFF"/>
-      <color rgb="FFFF66CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -322,7 +351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Story Points</c:v>
+                  <c:v>Story Points Completed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -944,7 +973,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -987,16 +1019,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1025,7 +1057,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="00FFFF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1068,16 +1100,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1106,7 +1138,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF66CC"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1152,13 +1184,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,10 +1480,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -2632,14 +2661,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
@@ -2969,7 +2998,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10:M11"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2999,7 +3028,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3016,7 +3045,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>37</v>
@@ -3048,7 +3077,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="H26" activeCellId="1" sqref="N9 H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,64 +3107,65 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <f>'Effort Description'!C26</f>
-        <v>40</v>
+        <f>'Effort Descriptions'!C26</f>
+        <v>14</v>
       </c>
       <c r="C2">
-        <f>'Effort Description'!D26</f>
-        <v>85</v>
+        <f>'Effort Descriptions'!D26</f>
+        <v>16</v>
       </c>
       <c r="D2">
-        <f>'Effort Description'!E26</f>
-        <v>90</v>
+        <f>'Effort Descriptions'!E26</f>
+        <v>18</v>
       </c>
       <c r="E2">
-        <f>'Effort Description'!F26</f>
-        <v>85</v>
+        <f>'Effort Descriptions'!F26</f>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <f>'Effort Description'!C16</f>
-        <v>0</v>
+        <f>'Effort Descriptions'!C16</f>
+        <v>10</v>
       </c>
       <c r="C3">
-        <f>'Effort Description'!D16</f>
-        <v>55</v>
+        <f>'Effort Descriptions'!D16</f>
+        <v>20</v>
       </c>
       <c r="D3">
-        <f>'Effort Description'!E16</f>
-        <v>90</v>
+        <f>'Effort Descriptions'!E16</f>
+        <v>22</v>
       </c>
       <c r="E3">
-        <f>'Effort Description'!F16</f>
-        <v>90</v>
+        <f>'Effort Descriptions'!F16</f>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
+        <f>'Effort Descriptions'!C8</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f>'Effort Description'!D8</f>
-        <v>60</v>
+        <f>'Effort Descriptions'!D8</f>
+        <v>20</v>
       </c>
       <c r="D4">
-        <f>'Effort Description'!E8</f>
-        <v>70</v>
+        <f>'Effort Descriptions'!E8</f>
+        <v>11</v>
       </c>
       <c r="E4">
-        <f>'Effort Description'!F8</f>
-        <v>85</v>
+        <f>'Effort Descriptions'!F8</f>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3145,42 +3175,445 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1E3F19-9C45-4B9F-B330-DAB5EFF49D53}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <f>SUM(D2:D5)</f>
+        <v>20</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" ref="E8:H8" si="0">SUM(E2:E5)</f>
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4">
+        <f>SUM(C12:C14)</f>
+        <v>10</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" ref="D16:H16" si="1">SUM(D12:D14)</f>
+        <v>20</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5">
+        <v>14</v>
+      </c>
+      <c r="D20" s="5">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5">
+        <v>14</v>
+      </c>
+      <c r="F20" s="5">
+        <v>14</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>4</v>
+      </c>
+      <c r="F21" s="5">
+        <v>8</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6">
+        <f>SUM(C20:C24)</f>
+        <v>14</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" ref="D26:H26" si="2">SUM(D20:D24)</f>
+        <v>16</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1A154D-3B45-42BA-8F85-7C0815483A0E}">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1">
@@ -3200,7 +3633,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
@@ -3220,7 +3653,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
@@ -3240,7 +3673,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -3280,7 +3713,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
@@ -3309,7 +3742,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3321,7 +3754,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -3341,7 +3774,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3361,7 +3794,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
@@ -3391,7 +3824,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -3421,7 +3854,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3433,7 +3866,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5">
@@ -3453,7 +3886,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5">
@@ -3473,7 +3906,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5">
@@ -3493,7 +3926,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5">
@@ -3513,7 +3946,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5">
@@ -3543,7 +3976,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6">

</xml_diff>

<commit_message>
Burnup Chart updated. Do not refer to others
</commit_message>
<xml_diff>
--- a/Chart.xlsx
+++ b/Chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanf\Desktop\School\Sem 3.2\ETI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0B8A64-D27F-4948-9E68-C55BB17A4459}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EA501C-8277-4ED7-AF4E-93EB88C6570C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2730" windowWidth="22545" windowHeight="12315" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10170" yWindow="2850" windowWidth="22545" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BurnUp Chart" sheetId="1" r:id="rId1"/>
-    <sheet name="Effort Chart" sheetId="2" r:id="rId2"/>
-    <sheet name="Effort Descriptions" sheetId="4" r:id="rId3"/>
+    <sheet name="NIL" sheetId="2" r:id="rId2"/>
+    <sheet name="misc" sheetId="4" r:id="rId3"/>
     <sheet name="do not refer" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>Sprint</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Test Cases Passed (Unit)</t>
+  </si>
+  <si>
+    <t>Total Effort:</t>
+  </si>
+  <si>
+    <t>Time taken / Number of Test Cases</t>
   </si>
 </sst>
 </file>
@@ -412,6 +418,48 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1614401858304297E-2"/>
+                  <c:y val="2.3738872403560759E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-593D-4BCF-905D-00D4359E43A1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.5171296388147688E-17"/>
+                  <c:y val="1.9782393669633955E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-593D-4BCF-905D-00D4359E43A1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -513,6 +561,12 @@
                 <c:pt idx="3">
                   <c:v>28</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -568,6 +622,27 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-5458-4729-8949-A227F3945658}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.878048780487796E-2"/>
+                  <c:y val="-2.7695351137487636E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-10C8-41F5-A05C-53A9059CD8F6}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -672,10 +747,10 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,7 +1037,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Effort Chart'!$A$2</c:f>
+              <c:f>NIL!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -988,7 +1063,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Effort Chart'!$B$1:$G$1</c:f>
+              <c:f>NIL!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1015,7 +1090,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Effort Chart'!$B$2:$G$2</c:f>
+              <c:f>NIL!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1046,7 +1121,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Effort Chart'!$A$3</c:f>
+              <c:f>NIL!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1069,7 +1144,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Effort Chart'!$B$1:$G$1</c:f>
+              <c:f>NIL!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1096,7 +1171,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Effort Chart'!$B$3:$G$3</c:f>
+              <c:f>NIL!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1127,7 +1202,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Effort Chart'!$A$4</c:f>
+              <c:f>NIL!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1150,7 +1225,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Effort Chart'!$B$1:$G$1</c:f>
+              <c:f>NIL!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1177,7 +1252,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Effort Chart'!$B$4:$G$4</c:f>
+              <c:f>NIL!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2998,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,6 +3118,12 @@
       <c r="E2">
         <v>28</v>
       </c>
+      <c r="F2">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3061,10 +3142,11 @@
         <v>37</v>
       </c>
       <c r="F3">
-        <v>37</v>
+        <f>37+24</f>
+        <v>61</v>
       </c>
       <c r="G3">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3078,7 +3160,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,19 +3193,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f>'Effort Descriptions'!D26</f>
+        <f>misc!D26</f>
         <v>14</v>
       </c>
       <c r="C2">
-        <f>'Effort Descriptions'!E26</f>
+        <f>misc!E26</f>
         <v>16</v>
       </c>
       <c r="D2">
-        <f>'Effort Descriptions'!F26</f>
+        <f>misc!F26</f>
         <v>18</v>
       </c>
       <c r="E2">
-        <f>'Effort Descriptions'!G26</f>
+        <f>misc!G26</f>
         <v>22</v>
       </c>
     </row>
@@ -3132,19 +3214,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f>'Effort Descriptions'!D16</f>
+        <f>misc!D16</f>
         <v>10</v>
       </c>
       <c r="C3">
-        <f>'Effort Descriptions'!E16</f>
+        <f>misc!E16</f>
         <v>20</v>
       </c>
       <c r="D3">
-        <f>'Effort Descriptions'!F16</f>
+        <f>misc!F16</f>
         <v>22</v>
       </c>
       <c r="E3">
-        <f>'Effort Descriptions'!G16</f>
+        <f>misc!G16</f>
         <v>9</v>
       </c>
     </row>
@@ -3153,19 +3235,19 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <f>'Effort Descriptions'!D8</f>
+        <f>misc!D8</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f>'Effort Descriptions'!E8</f>
+        <f>misc!E8</f>
         <v>20</v>
       </c>
       <c r="D4">
-        <f>'Effort Descriptions'!F8</f>
+        <f>misc!F8</f>
         <v>11</v>
       </c>
       <c r="E4">
-        <f>'Effort Descriptions'!G8</f>
+        <f>misc!G8</f>
         <v>27</v>
       </c>
     </row>
@@ -3179,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1E3F19-9C45-4B9F-B330-DAB5EFF49D53}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3235,7 +3317,9 @@
       <c r="G2" s="1">
         <v>11</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -3256,8 +3340,16 @@
       <c r="G3" s="1">
         <v>16</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
       <c r="I3" s="1"/>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -3326,7 +3418,7 @@
       </c>
       <c r="H8" s="2">
         <f>SUM(H2:H5)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2">
         <f>SUM(I2:I5)</f>
@@ -3376,7 +3468,9 @@
       <c r="G12" s="3">
         <v>5</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3397,7 +3491,9 @@
       <c r="G13" s="3">
         <v>4</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3">
+        <v>4</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3446,7 +3542,7 @@
       </c>
       <c r="H16" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="0"/>
@@ -3517,7 +3613,9 @@
       <c r="G21" s="5">
         <v>8</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Timeline and Charts #2
</commit_message>
<xml_diff>
--- a/Chart.xlsx
+++ b/Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanf\Desktop\School\Sem 3.2\ETI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D626A5-74B9-48EE-B78A-580BACF17C19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA63C4-C4FD-4AB7-9051-CF15EB736B4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10170" yWindow="2850" windowWidth="22545" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -389,19 +389,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1690,7 +1690,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,19 +1729,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>